<commit_message>
Created some example CSV files and config files for testing
</commit_message>
<xml_diff>
--- a/data_architect_misc/data_transformer/examples/excel2.xlsx
+++ b/data_architect_misc/data_transformer/examples/excel2.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lache\Documents\GitHub\others\data_architect_misc\data_transformer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lache\Documents\GitHub\others\data_architect_misc\data_transformer\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE10301-F0A9-47FF-8CF2-999715C2A599}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD782ED-ACC1-4D5B-80A5-AE6CDD0FBB38}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43290" yWindow="-990" windowWidth="17730" windowHeight="15585" xr2:uid="{FCEE7782-9213-40EB-9AC9-83CEA33A3CB2}"/>
+    <workbookView xWindow="32310" yWindow="1500" windowWidth="16530" windowHeight="10155" xr2:uid="{FCEE7782-9213-40EB-9AC9-83CEA33A3CB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -637,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1926ABE5-D524-4E85-AFBD-07C0DBC01CAF}">
-  <dimension ref="A2:E29"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,416 +652,416 @@
     <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>1</v>
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>6</v>
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="A6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="6" t="s">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>1</v>
+      <c r="A8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>11</v>
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>16</v>
+      <c r="A10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>21</v>
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>26</v>
+      <c r="A12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>31</v>
+      <c r="A13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>36</v>
+      <c r="A14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>41</v>
+      <c r="A15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>46</v>
+      <c r="A16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="5" t="s">
+      <c r="A17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>51</v>
+      <c r="C17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>55</v>
+      <c r="A18" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>60</v>
+      <c r="A19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>65</v>
+      <c r="A20" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" s="3" t="s">
+      <c r="A21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E26" s="6" t="s">
+      <c r="A26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="A27" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>